<commit_message>
notes about the disadvantages of some websites in getting xpath or article link - updated
</commit_message>
<xml_diff>
--- a/crawlingdata.xlsx
+++ b/crawlingdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Bộ/ Ngành</t>
   </si>
@@ -154,22 +154,138 @@
     <t>http://cema.gov.vn/home.htm</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xpath của mỗi link tin tức khác nhau ở chỗ t tô đỏ á :( //*[@id="BodyContent_ctl00_ctl00_rptStoryLineThumbnail_divItemSmall_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"]/div[1]/a</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve"> Ngân hàng Nhà nước Việt Nam</t>
   </si>
   <si>
     <t>https://www.sbv.gov.vn/webcenter/portal/vi/menu/trangchu;jsessionid=F5X8390vySpcPZ7QrftzbhKbWebL3_-GSPGOln8XcoOOq_7SYsV_!1777602058!103147707?_afrLoop=21080536281629224#%40%3F_afrLoop%3D21080536281629224%26centerWidth%3D80%2525%26leftWidth%3D10%2525%26rightWidth%3D10%2525%26showFooter%3Dfalse%26showHeader%3Dfalse%26_adf.ctrl-state%3D1afvgqb405_4</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//*[@id="T:oc_9259810424region:j_id__ctru19pc8:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:i1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:gl3"]</t>
+    </r>
+  </si>
+  <si>
     <t>Văn phòng Chính phủ</t>
   </si>
   <si>
     <t>http://vpcp.chinhphu.vn/</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>//*[@id="ctl00_bodyContent_ctl00___rptMainList_ctl0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>_lnkHeadline"]</t>
+    </r>
+  </si>
+  <si>
     <t>Bảo hiểm Xã hội Việt Nam</t>
   </si>
   <si>
     <t>https://baohiemxahoi.gov.vn/Pages/default.aspx</t>
+  </si>
+  <si>
+    <t>có xpath nhưng t chạy code không ra link, t lấy cả thẻ p và thẻ a</t>
   </si>
   <si>
     <t>Viện Hàn lâm Khoa học và Công nghệ Việt Nam</t>
@@ -200,7 +316,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,59 +333,118 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -291,52 +466,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -354,32 +483,38 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -391,55 +526,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -451,127 +676,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -582,6 +717,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -596,26 +755,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -647,8 +786,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -668,24 +807,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -703,132 +838,132 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -839,16 +974,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1170,8 +1307,8 @@
   <sheetPr/>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1200,7 +1337,7 @@
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1208,7 +1345,7 @@
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1216,7 +1353,7 @@
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1224,7 +1361,7 @@
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
@@ -1235,7 +1372,7 @@
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1243,7 +1380,7 @@
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1251,7 +1388,7 @@
       <c r="A9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1259,7 +1396,7 @@
       <c r="A10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1267,7 +1404,7 @@
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C11" t="s">
@@ -1278,7 +1415,7 @@
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1286,7 +1423,7 @@
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="C13" t="s">
@@ -1297,7 +1434,7 @@
       <c r="A14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
@@ -1308,7 +1445,7 @@
       <c r="A15" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="7" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1316,7 +1453,7 @@
       <c r="A16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1324,7 +1461,7 @@
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1332,7 +1469,7 @@
       <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="7" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1340,7 +1477,7 @@
       <c r="A19" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1348,64 +1485,76 @@
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:3">
       <c r="A21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>46</v>
       </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="9" t="s">
+        <v>47</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>48</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>50</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1442,12 +1591,15 @@
     <hyperlink ref="B13" r:id="rId30" display="https://www.mof.gov.vn/webcenter/portal/btc?_afrLoop=604986911223584#%40%3F_afrLoop%3D604986911223584%26_adf.ctrl-state%3Du42aoybdh_206" tooltip="https://www.mof.gov.vn/webcenter/portal/btc?_afrLoop=604986911223584#%40%3F_afrLoop%3D604986911223584%26_adf.ctrl-state%3Du42aoybdh_206"/>
     <hyperlink ref="B14" r:id="rId31" display="https://monre.gov.vn/" tooltip="https://monre.gov.vn/"/>
     <hyperlink ref="B15" r:id="rId32" display="https://www.mic.gov.vn/mic_2020/Pages/trangchu_2020.aspx"/>
-    <hyperlink ref="B16" r:id="rId33" display="https://moj.gov.vn/Pages/home.aspx"/>
-    <hyperlink ref="B18" r:id="rId34" display="https://moc.gov.vn/vn/Pages/Trangchu.aspx"/>
-    <hyperlink ref="B20" r:id="rId35" display="http://chinhphu.vn/portal/page/portal/chinhphu/trangchu"/>
-    <hyperlink ref="B21" r:id="rId36" display="http://cema.gov.vn/home.htm"/>
-    <hyperlink ref="B22" r:id="rId37" display="https://www.sbv.gov.vn/webcenter/portal/vi/menu/trangchu;jsessionid=F5X8390vySpcPZ7QrftzbhKbWebL3_-GSPGOln8XcoOOq_7SYsV_!1777602058!103147707?_afrLoop=21080536281629224#%40%3F_afrLoop%3D21080536281629224%26centerWidth%3D80%2525%26leftWidth%3D10%2525%26rightWidth%3D10%2525%26showFooter%3Dfalse%26showHeader%3Dfalse%26_adf.ctrl-state%3D1afvgqb405_4"/>
+    <hyperlink ref="B16" r:id="rId33" display="https://moj.gov.vn/Pages/home.aspx" tooltip="https://moj.gov.vn/Pages/home.aspx"/>
+    <hyperlink ref="B18" r:id="rId34" display="https://moc.gov.vn/vn/Pages/Trangchu.aspx" tooltip="https://moc.gov.vn/vn/Pages/Trangchu.aspx"/>
+    <hyperlink ref="B20" r:id="rId35" display="http://chinhphu.vn/portal/page/portal/chinhphu/trangchu" tooltip="http://chinhphu.vn/portal/page/portal/chinhphu/trangchu"/>
+    <hyperlink ref="B21" r:id="rId36" display="http://cema.gov.vn/home.htm" tooltip="http://cema.gov.vn/home.htm"/>
+    <hyperlink ref="B22" r:id="rId37" display="https://www.sbv.gov.vn/webcenter/portal/vi/menu/trangchu;jsessionid=F5X8390vySpcPZ7QrftzbhKbWebL3_-GSPGOln8XcoOOq_7SYsV_!1777602058!103147707?_afrLoop=21080536281629224#%40%3F_afrLoop%3D21080536281629224%26centerWidth%3D80%2525%26leftWidth%3D10%2525%26rightWidth%3D10%2525%26showFooter%3Dfalse%26showHeader%3Dfalse%26_adf.ctrl-state%3D1afvgqb405_4" tooltip="https://www.sbv.gov.vn/webcenter/portal/vi/menu/trangchu;jsessionid=F5X8390vySpcPZ7QrftzbhKbWebL3_-GSPGOln8XcoOOq_7SYsV_!1777602058!103147707?_afrLoop=21080536281629224#%40%3F_afrLoop%3D21080536281629224%26centerWidth%3D80%2525%26leftWidth%3D10%2525%26rig"/>
     <hyperlink ref="B2" r:id="rId38" display="http://www.moit.gov.vn/web/guest"/>
+    <hyperlink ref="B23" r:id="rId39" display="http://vpcp.chinhphu.vn/"/>
+    <hyperlink ref="B24" r:id="rId40" display="https://baohiemxahoi.gov.vn/Pages/default.aspx"/>
+    <hyperlink ref="B25" r:id="rId41" display="https://vast.gov.vn/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
Update table category_info and other related tables. Update notes in crawlingdata.xlxs
</commit_message>
<xml_diff>
--- a/crawlingdata.xlsx
+++ b/crawlingdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="11520" windowHeight="9192"/>
+    <workbookView windowWidth="23040" windowHeight="9335"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
   <si>
     <t>Bộ/ Ngành</t>
   </si>
@@ -22,6 +22,12 @@
     <t>Link</t>
   </si>
   <si>
+    <t>ministry_category_configuration</t>
+  </si>
+  <si>
+    <t>category_info</t>
+  </si>
+  <si>
     <t>Bộ Công Thương</t>
   </si>
   <si>
@@ -55,6 +61,9 @@
     <t>không có mục tin tức, lấy tin từ trang chủ</t>
   </si>
   <si>
+    <t>Không có mục tin tức</t>
+  </si>
+  <si>
     <t>Bộ Khoa học và Công nghệ</t>
   </si>
   <si>
@@ -67,6 +76,9 @@
     <t>http://www.molisa.gov.vn/Pages/trangchu.aspx</t>
   </si>
   <si>
+    <t>mục nhỏ ở từng mục phân loại khá là nhiều</t>
+  </si>
+  <si>
     <t>Bộ Ngoại giao</t>
   </si>
   <si>
@@ -79,6 +91,9 @@
     <t>https://www.moha.gov.vn/</t>
   </si>
   <si>
+    <t>không thấy mục tin tức</t>
+  </si>
+  <si>
     <t>Bộ Nông nghiệp và Phát triển nông thôn</t>
   </si>
   <si>
@@ -88,12 +103,18 @@
     <t>lấy ảnh bị lỗi - tạm thời bỏ qua</t>
   </si>
   <si>
+    <t>cần thêm category type</t>
+  </si>
+  <si>
     <t>Bộ Quốc phòng</t>
   </si>
   <si>
     <t>http://www.mod.gov.vn/wps/portal</t>
   </si>
   <si>
+    <t>có nhiều category trong mục tin tức sự kiện, cân nhắc thêm category_type</t>
+  </si>
+  <si>
     <t>Bộ Tài chính</t>
   </si>
   <si>
@@ -112,12 +133,18 @@
     <t>không lấy tin chuyên ngành và tin địa phương vì xpath khác quá trời hic, 2 mục còn lại có xpath nhưng khum lấy link article được t nghĩ vì cái start_url nó như này hic https://monre.gov.vn/Pages/ChuyenMuc.aspx?cm=H%E1%BB%99i%20nh%E1%BA%ADp%20qu%E1%BB%91c%20t%E1%BA%BF</t>
   </si>
   <si>
+    <t>chưa kéo tới cuối trang đượt</t>
+  </si>
+  <si>
     <t>Bộ Thông tin và Truyền thông</t>
   </si>
   <si>
     <t>https://www.mic.gov.vn/mic_2020/Pages/trangchu_2020.aspx</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.mic.gov.vn/mic_2020/Pages/ChuyenMuc/PhanTrang/1748/3/Vien-thong.html - số trang nằm ở giữa </t>
+  </si>
+  <si>
     <t>Bộ Tư pháp</t>
   </si>
   <si>
@@ -130,6 +157,9 @@
     <t>https://bvhttdl.gov.vn/</t>
   </si>
   <si>
+    <t>https://bvhttdl.gov.vn/tin-tuc-va-su-kien/trang-3.htm - lại là số trang :&lt;</t>
+  </si>
+  <si>
     <t>Bộ Xây dựng</t>
   </si>
   <si>
@@ -142,10 +172,16 @@
     <t>https://moh.gov.vn/</t>
   </si>
   <si>
+    <t>không thấy mục tin tức =&gt; thêm field nhỏ bên trong từng mục</t>
+  </si>
+  <si>
     <t>Chính phủ</t>
   </si>
   <si>
     <t>http://chinhphu.vn/portal/page/portal/chinhphu/trangchu</t>
+  </si>
+  <si>
+    <t>*lấy tin từ phần tin nổi bật</t>
   </si>
   <si>
     <t>Ủy ban Dân tộc</t>
@@ -311,10 +347,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -375,9 +411,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -387,43 +438,6 @@
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -466,6 +480,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -474,13 +502,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -489,16 +525,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -517,7 +553,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,25 +562,199 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.35"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,157 +766,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -717,30 +777,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -783,15 +819,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -809,6 +836,39 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -820,15 +880,15 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -839,152 +899,159 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1305,256 +1372,310 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="39.6666666666667" style="2" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
+    <col min="3" max="3" width="37.4537037037037" customWidth="1"/>
+    <col min="4" max="4" width="49.2037037037037" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:2">
+    <row r="1" s="1" customFormat="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>43</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>48</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>50</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="9" t="s">
-        <v>47</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="14" t="s">
+        <v>59</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>60</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>52</v>
+        <v>62</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
+        <v>65</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>68</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>70</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1600,6 +1721,8 @@
     <hyperlink ref="B23" r:id="rId39" display="http://vpcp.chinhphu.vn/"/>
     <hyperlink ref="B24" r:id="rId40" display="https://baohiemxahoi.gov.vn/Pages/default.aspx"/>
     <hyperlink ref="B25" r:id="rId41" display="https://vast.gov.vn/"/>
+    <hyperlink ref="D15" r:id="rId42" display="https://www.mic.gov.vn/mic_2020/Pages/ChuyenMuc/PhanTrang/1748/3/Vien-thong.html - số trang nằm ở giữa "/>
+    <hyperlink ref="D17" r:id="rId43" display="https://bvhttdl.gov.vn/tin-tuc-va-su-kien/trang-3.htm - lại là số trang :&lt;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>

<commit_message>
add tables: legislationinfo, legislation_type and insert data
</commit_message>
<xml_diff>
--- a/crawlingdata.xlsx
+++ b/crawlingdata.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="78">
   <si>
     <t>Bộ/ Ngành</t>
   </si>
@@ -64,12 +64,18 @@
     <t>Không có mục tin tức</t>
   </si>
   <si>
+    <t>lấy văn bản bị crash - lấy được gòi</t>
+  </si>
+  <si>
     <t>Bộ Khoa học và Công nghệ</t>
   </si>
   <si>
     <t>https://www.most.gov.vn/vn/Pages/Trangchu.aspx</t>
   </si>
   <si>
+    <t>đang lấy cái crash tức ghê</t>
+  </si>
+  <si>
     <t>Bộ Lao động - Thương Binh và Xã hội</t>
   </si>
   <si>
@@ -106,6 +112,9 @@
     <t>cần thêm category type</t>
   </si>
   <si>
+    <t>nó không có ở trong trang khác í</t>
+  </si>
+  <si>
     <t>Bộ Quốc phòng</t>
   </si>
   <si>
@@ -173,6 +182,9 @@
   </si>
   <si>
     <t>không thấy mục tin tức =&gt; thêm field nhỏ bên trong từng mục</t>
+  </si>
+  <si>
+    <t>Phải đăng nhập mới xem được văn bản</t>
   </si>
   <si>
     <t>Chính phủ</t>
@@ -347,9 +359,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
@@ -405,45 +417,38 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,20 +485,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -504,20 +495,49 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -526,15 +546,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -592,6 +604,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -604,7 +652,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,157 +754,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -777,6 +789,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -819,6 +846,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -836,24 +872,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -866,21 +889,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -899,140 +911,137 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
@@ -1372,13 +1381,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.83333333333333" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="39.6666666666667" style="2" customWidth="1"/>
     <col min="2" max="2" width="61.5" customWidth="1"/>
@@ -1387,16 +1396,16 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1404,278 +1413,290 @@
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:5">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>22</v>
+      <c r="A9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="7" t="s">
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>32</v>
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
-      <c r="A13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>35</v>
+      <c r="A13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="10" t="s">
+      <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="B14" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>42</v>
+      <c r="A15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>44</v>
+      <c r="A16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>47</v>
+      <c r="A17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="A18" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="B18" s="3" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>25</v>
+        <v>59</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="13"/>
+        <v>60</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" s="12"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>25</v>
+      <c r="A22" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>25</v>
+        <v>66</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>69</v>
+        <v>72</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>25</v>
+        <v>74</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>25</v>
+        <v>76</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>